<commit_message>
completed 3 sections of formula based formatting
</commit_message>
<xml_diff>
--- a/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
+++ b/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\SecondLens\Excel Maven\Udemy\Course 1 - Formulas &amp; Functions\FINAL Resource Docs\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Demo Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB92339-C917-144E-949A-40489175282E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Checker Example" sheetId="4" r:id="rId1"/>
     <sheet name="State Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -237,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -466,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,7 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,9 +529,6 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,19 +538,17 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,9 +560,34 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -833,26 +862,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="7"/>
-    <col min="2" max="2" width="11.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="7"/>
+    <col min="1" max="1" width="9.1640625" style="7"/>
+    <col min="2" max="2" width="11.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
         <v>55</v>
       </c>
@@ -869,7 +898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>60</v>
       </c>
@@ -889,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>61</v>
       </c>
@@ -909,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>62</v>
       </c>
@@ -929,7 +958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>63</v>
       </c>
@@ -949,69 +978,70 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>30</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>31</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>32</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>33</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24" t="s">
+    <row r="9" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="27">
         <f>INDEX(C3:G7,MATCH(B10,B3:B7,0),MATCH(C10,C2:G2,0))</f>
-        <v>25</v>
-      </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="28"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:G7">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>C3=$E$10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$B$3:$B$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$C$2:$G$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1020,17 +1050,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
@@ -1038,7 +1068,7 @@
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1096,7 @@
         <v>948435</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1080,7 +1110,7 @@
         <v>67228.56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1124,7 @@
         <v>1396668.64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1138,7 @@
         <v>257943</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1122,7 +1152,7 @@
         <v>8492127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +1166,7 @@
         <v>1226556.08</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1180,7 @@
         <v>870963.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1164,7 +1194,7 @@
         <v>166161</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1178,7 +1208,7 @@
         <v>74619.08</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1222,7 @@
         <v>2563588.48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1206,7 +1236,7 @@
         <v>424630.65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1220,7 +1250,7 @@
         <v>350042.36000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1234,7 +1264,7 @@
         <v>77162.649999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1248,7 +1278,7 @@
         <v>1493403.16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1262,7 +1292,7 @@
         <v>935648.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1276,7 +1306,7 @@
         <v>282183.15999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1290,7 +1320,7 @@
         <v>520793.42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1304,7 +1334,7 @@
         <v>1180743.01</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1348,7 @@
         <v>626278.64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1362,7 @@
         <v>223195.91</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1346,7 +1376,7 @@
         <v>1399498.36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1360,7 +1390,7 @@
         <v>1348044.3699999999</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1404,7 @@
         <v>1014215.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1418,7 @@
         <v>1195974.96</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1432,7 @@
         <v>163632.9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1416,7 +1446,7 @@
         <v>737321.43</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1430,7 +1460,7 @@
         <v>208951.94999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1444,7 +1474,7 @@
         <v>433519.12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1458,7 +1488,7 @@
         <v>454378.54</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1472,7 +1502,7 @@
         <v>333845.36</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1486,7 +1516,7 @@
         <v>2380883</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1500,7 +1530,7 @@
         <v>562865.79999999993</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1514,7 +1544,7 @@
         <v>3423896.26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1528,7 +1558,7 @@
         <v>1305166.08</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -1542,7 +1572,7 @@
         <v>91162</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -1556,7 +1586,7 @@
         <v>3184585.2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -1570,7 +1600,7 @@
         <v>265244.78000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1614,7 @@
         <v>257362.93000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1598,7 +1628,7 @@
         <v>2108095.1800000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v>171151.85</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -1626,7 +1656,7 @@
         <v>411020.2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -1640,7 +1670,7 @@
         <v>102596.72</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -1654,7 +1684,7 @@
         <v>634265.13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1668,7 +1698,7 @@
         <v>2299911.2000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1682,7 +1712,7 @@
         <v>388384.73000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1696,7 +1726,7 @@
         <v>159402.47999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1710,7 +1740,7 @@
         <v>1438739</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1724,7 +1754,7 @@
         <v>1371305.83</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1738,7 +1768,7 @@
         <v>533269.76000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1752,7 +1782,7 @@
         <v>1415260.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
completed first 3 sections of formula formatting
</commit_message>
<xml_diff>
--- a/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
+++ b/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Demo Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB92339-C917-144E-949A-40489175282E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5880E425-F165-F24F-886D-07E1F1F6EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Checker Example" sheetId="4" r:id="rId1"/>
     <sheet name="State Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -562,15 +565,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -579,11 +578,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -869,7 +868,7 @@
   <dimension ref="B1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1012,7 +1011,7 @@
     </row>
     <row r="10" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>59</v>
@@ -1022,7 +1021,7 @@
       </c>
       <c r="E10" s="27">
         <f>INDEX(C3:G7,MATCH(B10,B3:B7,0),MATCH(C10,C2:G2,0))</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="25"/>
@@ -1057,7 +1056,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
completed formula formatting section
</commit_message>
<xml_diff>
--- a/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
+++ b/Excel Demo Workbooks/Section8_Formula_Formatting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel Demo Workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5880E425-F165-F24F-886D-07E1F1F6EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149FEA6F-4C8A-7142-A48D-895B829A1FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Checker Example" sheetId="4" r:id="rId1"/>
@@ -474,11 +474,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,12 +561,127 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -867,8 +983,8 @@
   </sheetPr>
   <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1148,7 @@
     <mergeCell ref="E10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:G7">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>C3=$E$10</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1053,10 +1169,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1067,7 +1183,7 @@
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1197,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1094,8 +1210,9 @@
       <c r="D2" s="6">
         <v>948435</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1108,8 +1225,9 @@
       <c r="D3" s="6">
         <v>67228.56</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1122,8 +1240,9 @@
       <c r="D4" s="6">
         <v>1396668.64</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1136,8 +1255,9 @@
       <c r="D5" s="6">
         <v>257943</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1150,8 +1270,9 @@
       <c r="D6" s="6">
         <v>8492127</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1164,8 +1285,9 @@
       <c r="D7" s="6">
         <v>1226556.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1178,8 +1300,9 @@
       <c r="D8" s="6">
         <v>870963.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1192,8 +1315,9 @@
       <c r="D9" s="6">
         <v>166161</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1206,8 +1330,9 @@
       <c r="D10" s="6">
         <v>74619.08</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1220,8 +1345,9 @@
       <c r="D11" s="6">
         <v>2563588.48</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1234,8 +1360,9 @@
       <c r="D12" s="6">
         <v>424630.65</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1248,8 +1375,9 @@
       <c r="D13" s="6">
         <v>350042.36000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1262,8 +1390,9 @@
       <c r="D14" s="6">
         <v>77162.649999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1276,8 +1405,9 @@
       <c r="D15" s="6">
         <v>1493403.16</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1290,8 +1420,9 @@
       <c r="D16" s="6">
         <v>935648.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1304,8 +1435,9 @@
       <c r="D17" s="6">
         <v>282183.15999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1318,8 +1450,9 @@
       <c r="D18" s="6">
         <v>520793.42</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1332,8 +1465,9 @@
       <c r="D19" s="6">
         <v>1180743.01</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1346,8 +1480,9 @@
       <c r="D20" s="6">
         <v>626278.64</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1360,8 +1495,9 @@
       <c r="D21" s="6">
         <v>223195.91</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1374,8 +1510,9 @@
       <c r="D22" s="6">
         <v>1399498.36</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1388,8 +1525,9 @@
       <c r="D23" s="6">
         <v>1348044.3699999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1402,8 +1540,9 @@
       <c r="D24" s="6">
         <v>1014215.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1416,8 +1555,9 @@
       <c r="D25" s="6">
         <v>1195974.96</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1430,8 +1570,9 @@
       <c r="D26" s="6">
         <v>163632.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1444,8 +1585,9 @@
       <c r="D27" s="6">
         <v>737321.43</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1458,8 +1600,9 @@
       <c r="D28" s="6">
         <v>208951.94999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1472,8 +1615,9 @@
       <c r="D29" s="6">
         <v>433519.12</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1486,8 +1630,9 @@
       <c r="D30" s="6">
         <v>454378.54</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1500,8 +1645,9 @@
       <c r="D31" s="6">
         <v>333845.36</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1514,8 +1660,9 @@
       <c r="D32" s="6">
         <v>2380883</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1528,8 +1675,9 @@
       <c r="D33" s="6">
         <v>562865.79999999993</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1542,8 +1690,9 @@
       <c r="D34" s="6">
         <v>3423896.26</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="29"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1556,8 +1705,9 @@
       <c r="D35" s="6">
         <v>1305166.08</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="29"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -1570,8 +1720,9 @@
       <c r="D36" s="6">
         <v>91162</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="29"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -1584,8 +1735,9 @@
       <c r="D37" s="6">
         <v>3184585.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -1598,8 +1750,9 @@
       <c r="D38" s="6">
         <v>265244.78000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -1612,8 +1765,9 @@
       <c r="D39" s="6">
         <v>257362.93000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="29"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1626,8 +1780,9 @@
       <c r="D40" s="6">
         <v>2108095.1800000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="29"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1640,8 +1795,9 @@
       <c r="D41" s="6">
         <v>171151.85</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="29"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -1654,8 +1810,9 @@
       <c r="D42" s="6">
         <v>411020.2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="29"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -1668,8 +1825,9 @@
       <c r="D43" s="6">
         <v>102596.72</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="29"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -1682,8 +1840,9 @@
       <c r="D44" s="6">
         <v>634265.13</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="29"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1696,8 +1855,9 @@
       <c r="D45" s="6">
         <v>2299911.2000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="29"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1710,8 +1870,9 @@
       <c r="D46" s="6">
         <v>388384.73000000004</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="29"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1724,8 +1885,9 @@
       <c r="D47" s="6">
         <v>159402.47999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="29"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1738,8 +1900,9 @@
       <c r="D48" s="6">
         <v>1438739</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="29"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1752,8 +1915,9 @@
       <c r="D49" s="6">
         <v>1371305.83</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="29"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1766,8 +1930,9 @@
       <c r="D50" s="6">
         <v>533269.76000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="29"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1780,8 +1945,9 @@
       <c r="D51" s="6">
         <v>1415260.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="29"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -1794,8 +1960,14 @@
       <c r="D52" s="6">
         <v>95463.94</v>
       </c>
+      <c r="E52" s="29"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:D52">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(LEFT($A2,1)="I",RIGHT($A2,1)="a")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>